<commit_message>
Added Data driven Cases
</commit_message>
<xml_diff>
--- a/src/main/resources/ScanTestData.xlsx
+++ b/src/main/resources/ScanTestData.xlsx
@@ -8,26 +8,37 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Automation Setup\AST Automation\Automation\src\main\resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0B7714C1-41F9-4232-A0AF-4691B0FE7B75}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1C08779A-9F35-4CAA-A0A8-B442FAC2055B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="170" windowWidth="19200" windowHeight="11110" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="ScanSheet" sheetId="1" r:id="rId1"/>
+    <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="124519"/>
+  <calcPr calcId="191029"/>
+  <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
+      </xcalcf:calcFeatures>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="56" uniqueCount="28">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="84" uniqueCount="37">
   <si>
     <t>ScenarioDescription</t>
   </si>
   <si>
-    <t>Branch</t>
-  </si>
-  <si>
     <t>ScanTypes</t>
   </si>
   <si>
@@ -58,12 +69,6 @@
     <t>Full</t>
   </si>
   <si>
-    <t>ProjectNamePattern</t>
-  </si>
-  <si>
-    <t>CLI_ScanProj_</t>
-  </si>
-  <si>
     <t>ExpectedEngine</t>
   </si>
   <si>
@@ -104,6 +109,42 @@
   </si>
   <si>
     <t>ALL scan using local zip file</t>
+  </si>
+  <si>
+    <t>SAST scan with empty application name</t>
+  </si>
+  <si>
+    <t>SAST scan with valid application name</t>
+  </si>
+  <si>
+    <t>`--application-name "ShubhamApplicationForAutomation"</t>
+  </si>
+  <si>
+    <t>`--application-name ""</t>
+  </si>
+  <si>
+    <t>`--sast-fast-scan</t>
+  </si>
+  <si>
+    <t>SAST scan with sast-fast-scan flag</t>
+  </si>
+  <si>
+    <t>`--apikey %s</t>
+  </si>
+  <si>
+    <t>SAST scan with valid Api Key</t>
+  </si>
+  <si>
+    <t>`--client-id %s --client-secret %s</t>
+  </si>
+  <si>
+    <t>SAST scan with valid Client Secret</t>
+  </si>
+  <si>
+    <t>`--project-groups "QA Team"</t>
+  </si>
+  <si>
+    <t>SAST scan with valid Group Name</t>
   </si>
 </sst>
 </file>
@@ -162,12 +203,16 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
+    <xf numFmtId="49" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -472,206 +517,321 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:I7"/>
+  <dimension ref="A1:G13"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C6" sqref="C6"/>
+      <selection activeCell="A8" sqref="A8:G13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="28.90625" customWidth="1"/>
-    <col min="2" max="2" width="25.6328125" customWidth="1"/>
-    <col min="3" max="3" width="19.1796875" customWidth="1"/>
-    <col min="4" max="4" width="22.08984375" customWidth="1"/>
-    <col min="5" max="5" width="16.90625" customWidth="1"/>
-    <col min="6" max="6" width="12.81640625" customWidth="1"/>
+    <col min="1" max="1" width="35.90625" customWidth="1"/>
+    <col min="2" max="2" width="22.08984375" customWidth="1"/>
+    <col min="3" max="3" width="57.54296875" customWidth="1"/>
+    <col min="4" max="4" width="12.81640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" t="s">
+      <c r="B1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1" s="2" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A2" t="s">
+        <v>6</v>
+      </c>
+      <c r="B2" t="s">
+        <v>8</v>
+      </c>
+      <c r="D2" t="s">
+        <v>9</v>
+      </c>
+      <c r="E2" t="s">
+        <v>7</v>
+      </c>
+      <c r="F2" t="s">
+        <v>10</v>
+      </c>
+      <c r="G2" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A3" t="s">
         <v>12</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="D1" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="E1" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="F1" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="G1" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="H1" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="I1" s="2" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A2" t="s">
-        <v>7</v>
-      </c>
-      <c r="B2" t="s">
-        <v>13</v>
-      </c>
-      <c r="C2" t="s">
-        <v>8</v>
-      </c>
-      <c r="D2" t="s">
-        <v>9</v>
-      </c>
-      <c r="F2" t="s">
-        <v>10</v>
-      </c>
-      <c r="G2" t="s">
-        <v>8</v>
-      </c>
-      <c r="H2" t="s">
-        <v>11</v>
-      </c>
-      <c r="I2" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A3" t="s">
-        <v>15</v>
       </c>
       <c r="B3" t="s">
         <v>13</v>
       </c>
-      <c r="C3" t="s">
-        <v>8</v>
-      </c>
       <c r="D3" t="s">
+        <v>9</v>
+      </c>
+      <c r="E3" t="s">
+        <v>7</v>
+      </c>
+      <c r="F3" t="s">
+        <v>10</v>
+      </c>
+      <c r="G3" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A4" t="s">
         <v>16</v>
       </c>
-      <c r="F3" t="s">
-        <v>10</v>
-      </c>
-      <c r="G3" t="s">
-        <v>8</v>
-      </c>
-      <c r="H3" t="s">
-        <v>11</v>
-      </c>
-      <c r="I3" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A4" t="s">
+      <c r="B4" t="s">
+        <v>14</v>
+      </c>
+      <c r="D4" t="s">
+        <v>9</v>
+      </c>
+      <c r="E4" t="s">
+        <v>7</v>
+      </c>
+      <c r="F4" t="s">
+        <v>10</v>
+      </c>
+      <c r="G4" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A5" t="s">
         <v>19</v>
       </c>
-      <c r="B4" t="s">
-        <v>13</v>
-      </c>
-      <c r="C4" t="s">
-        <v>8</v>
-      </c>
-      <c r="D4" t="s">
+      <c r="B5" t="s">
         <v>17</v>
       </c>
-      <c r="F4" t="s">
-        <v>10</v>
-      </c>
-      <c r="G4" t="s">
-        <v>8</v>
-      </c>
-      <c r="H4" t="s">
-        <v>11</v>
-      </c>
-      <c r="I4" t="s">
+      <c r="D5" t="s">
+        <v>9</v>
+      </c>
+      <c r="E5" t="s">
+        <v>7</v>
+      </c>
+      <c r="F5" t="s">
+        <v>10</v>
+      </c>
+      <c r="G5" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A5" t="s">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A6" t="s">
+        <v>21</v>
+      </c>
+      <c r="B6" t="s">
+        <v>20</v>
+      </c>
+      <c r="D6" t="s">
+        <v>9</v>
+      </c>
+      <c r="E6" t="s">
+        <v>7</v>
+      </c>
+      <c r="F6" t="s">
+        <v>10</v>
+      </c>
+      <c r="G6" t="s">
         <v>22</v>
       </c>
-      <c r="B5" t="s">
-        <v>13</v>
-      </c>
-      <c r="C5" t="s">
-        <v>8</v>
-      </c>
-      <c r="D5" t="s">
-        <v>20</v>
-      </c>
-      <c r="F5" t="s">
-        <v>10</v>
-      </c>
-      <c r="G5" t="s">
-        <v>8</v>
-      </c>
-      <c r="H5" t="s">
-        <v>11</v>
-      </c>
-      <c r="I5" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A6" t="s">
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A7" t="s">
         <v>24</v>
       </c>
-      <c r="B6" t="s">
-        <v>13</v>
-      </c>
-      <c r="C6" t="s">
-        <v>8</v>
-      </c>
-      <c r="D6" t="s">
+      <c r="D7" t="s">
+        <v>9</v>
+      </c>
+      <c r="E7" t="s">
+        <v>7</v>
+      </c>
+      <c r="F7" t="s">
+        <v>10</v>
+      </c>
+      <c r="G7" t="s">
         <v>23</v>
       </c>
-      <c r="F6" t="s">
-        <v>10</v>
-      </c>
-      <c r="G6" t="s">
-        <v>8</v>
-      </c>
-      <c r="H6" t="s">
-        <v>11</v>
-      </c>
-      <c r="I6" t="s">
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A8" t="s">
         <v>25</v>
       </c>
-    </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A7" t="s">
+      <c r="B8" t="s">
+        <v>8</v>
+      </c>
+      <c r="C8" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="D8" t="s">
+        <v>9</v>
+      </c>
+      <c r="E8" t="s">
+        <v>7</v>
+      </c>
+      <c r="F8" t="s">
+        <v>10</v>
+      </c>
+      <c r="G8" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A9" t="s">
+        <v>26</v>
+      </c>
+      <c r="B9" t="s">
+        <v>8</v>
+      </c>
+      <c r="C9" s="3" t="s">
         <v>27</v>
       </c>
-      <c r="B7" t="s">
-        <v>13</v>
-      </c>
-      <c r="C7" t="s">
-        <v>8</v>
-      </c>
-      <c r="F7" t="s">
-        <v>10</v>
-      </c>
-      <c r="G7" t="s">
-        <v>8</v>
-      </c>
-      <c r="H7" t="s">
-        <v>11</v>
-      </c>
-      <c r="I7" t="s">
-        <v>26</v>
+      <c r="D9" t="s">
+        <v>9</v>
+      </c>
+      <c r="E9" t="s">
+        <v>7</v>
+      </c>
+      <c r="F9" t="s">
+        <v>10</v>
+      </c>
+      <c r="G9" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A10" t="s">
+        <v>30</v>
+      </c>
+      <c r="B10" t="s">
+        <v>8</v>
+      </c>
+      <c r="C10" t="s">
+        <v>29</v>
+      </c>
+      <c r="D10" t="s">
+        <v>9</v>
+      </c>
+      <c r="E10" t="s">
+        <v>7</v>
+      </c>
+      <c r="F10" t="s">
+        <v>10</v>
+      </c>
+      <c r="G10" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A11" t="s">
+        <v>32</v>
+      </c>
+      <c r="B11" t="s">
+        <v>8</v>
+      </c>
+      <c r="C11" t="s">
+        <v>31</v>
+      </c>
+      <c r="D11" t="s">
+        <v>9</v>
+      </c>
+      <c r="E11" t="s">
+        <v>7</v>
+      </c>
+      <c r="F11" t="s">
+        <v>10</v>
+      </c>
+      <c r="G11" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A12" t="s">
+        <v>34</v>
+      </c>
+      <c r="B12" t="s">
+        <v>8</v>
+      </c>
+      <c r="C12" t="s">
+        <v>33</v>
+      </c>
+      <c r="D12" t="s">
+        <v>9</v>
+      </c>
+      <c r="E12" t="s">
+        <v>7</v>
+      </c>
+      <c r="F12" t="s">
+        <v>10</v>
+      </c>
+      <c r="G12" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A13" t="s">
+        <v>36</v>
+      </c>
+      <c r="B13" t="s">
+        <v>8</v>
+      </c>
+      <c r="C13" t="s">
+        <v>35</v>
+      </c>
+      <c r="D13" t="s">
+        <v>9</v>
+      </c>
+      <c r="E13" t="s">
+        <v>7</v>
+      </c>
+      <c r="F13" t="s">
+        <v>10</v>
+      </c>
+      <c r="G13" t="s">
+        <v>8</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C5771A20-F90E-4137-B244-FA403CC5F2C0}">
+  <dimension ref="C8"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A2" sqref="A2:G7"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="3" max="3" width="76.81640625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="8" spans="3:3" x14ac:dyDescent="0.35">
+      <c r="C8" s="3"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Added all scan test
</commit_message>
<xml_diff>
--- a/src/main/resources/ScanTestData.xlsx
+++ b/src/main/resources/ScanTestData.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="29328"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="29426"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Automation Setup\AST Automation\Automation\src\main\resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3A78C49E-46EC-4CCB-9682-ACBC29916441}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4B3717C5-483A-4EE4-8255-67D91809CC82}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="890" windowWidth="19200" windowHeight="11110" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="ScanSheet" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="220" uniqueCount="85">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="215" uniqueCount="83">
   <si>
     <t>ScenarioDescription</t>
   </si>
@@ -103,12 +103,6 @@
   </si>
   <si>
     <t>containers</t>
-  </si>
-  <si>
-    <t>sast kics sca apisec containers scs</t>
-  </si>
-  <si>
-    <t>ALL scan using local zip file</t>
   </si>
   <si>
     <t>SAST scan with empty application name</t>
@@ -661,10 +655,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:H31"/>
+  <dimension ref="A1:H30"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A15" workbookViewId="0">
-      <selection activeCell="C25" sqref="C25"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C17" sqref="C17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -698,12 +692,12 @@
         <v>11</v>
       </c>
       <c r="H1" s="2" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="B2" t="s">
         <v>8</v>
@@ -724,13 +718,13 @@
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="B3" t="s">
         <v>8</v>
       </c>
       <c r="C3" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="D3" t="s">
         <v>9</v>
@@ -747,13 +741,13 @@
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="B4" t="s">
         <v>8</v>
       </c>
       <c r="C4" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="D4" t="s">
         <v>9</v>
@@ -870,7 +864,10 @@
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A10" t="s">
-        <v>24</v>
+        <v>43</v>
+      </c>
+      <c r="B10" t="s">
+        <v>44</v>
       </c>
       <c r="D10" t="s">
         <v>9</v>
@@ -882,15 +879,21 @@
         <v>10</v>
       </c>
       <c r="G10" t="s">
-        <v>23</v>
+        <v>8</v>
+      </c>
+      <c r="H10" t="s">
+        <v>45</v>
       </c>
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A11" t="s">
-        <v>45</v>
+        <v>29</v>
       </c>
       <c r="B11" t="s">
-        <v>46</v>
+        <v>8</v>
+      </c>
+      <c r="C11" t="s">
+        <v>28</v>
       </c>
       <c r="D11" t="s">
         <v>9</v>
@@ -903,20 +906,17 @@
       </c>
       <c r="G11" t="s">
         <v>8</v>
-      </c>
-      <c r="H11" t="s">
-        <v>47</v>
       </c>
     </row>
     <row r="12" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A12" t="s">
-        <v>31</v>
+        <v>38</v>
       </c>
       <c r="B12" t="s">
         <v>8</v>
       </c>
       <c r="C12" t="s">
-        <v>30</v>
+        <v>37</v>
       </c>
       <c r="D12" t="s">
         <v>9</v>
@@ -929,17 +929,20 @@
       </c>
       <c r="G12" t="s">
         <v>8</v>
+      </c>
+      <c r="H12" t="s">
+        <v>36</v>
       </c>
     </row>
     <row r="13" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A13" t="s">
-        <v>40</v>
+        <v>34</v>
       </c>
       <c r="B13" t="s">
         <v>8</v>
       </c>
       <c r="C13" t="s">
-        <v>39</v>
+        <v>33</v>
       </c>
       <c r="D13" t="s">
         <v>9</v>
@@ -952,20 +955,17 @@
       </c>
       <c r="G13" t="s">
         <v>8</v>
-      </c>
-      <c r="H13" t="s">
-        <v>38</v>
       </c>
     </row>
     <row r="14" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A14" t="s">
-        <v>36</v>
+        <v>46</v>
       </c>
       <c r="B14" t="s">
         <v>8</v>
       </c>
       <c r="C14" t="s">
-        <v>35</v>
+        <v>39</v>
       </c>
       <c r="D14" t="s">
         <v>9</v>
@@ -978,17 +978,20 @@
       </c>
       <c r="G14" t="s">
         <v>8</v>
+      </c>
+      <c r="H14" t="s">
+        <v>40</v>
       </c>
     </row>
     <row r="15" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A15" t="s">
-        <v>48</v>
+        <v>23</v>
       </c>
       <c r="B15" t="s">
         <v>8</v>
       </c>
-      <c r="C15" t="s">
-        <v>41</v>
+      <c r="C15" s="3" t="s">
+        <v>27</v>
       </c>
       <c r="D15" t="s">
         <v>9</v>
@@ -1001,20 +1004,17 @@
       </c>
       <c r="G15" t="s">
         <v>8</v>
-      </c>
-      <c r="H15" t="s">
-        <v>42</v>
       </c>
     </row>
     <row r="16" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A16" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B16" t="s">
         <v>8</v>
       </c>
       <c r="C16" s="3" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
       <c r="D16" t="s">
         <v>9</v>
@@ -1031,13 +1031,13 @@
     </row>
     <row r="17" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A17" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B17" t="s">
         <v>8</v>
       </c>
       <c r="C17" s="3" t="s">
-        <v>28</v>
+        <v>41</v>
       </c>
       <c r="D17" t="s">
         <v>9</v>
@@ -1050,17 +1050,20 @@
       </c>
       <c r="G17" t="s">
         <v>8</v>
+      </c>
+      <c r="H17" t="s">
+        <v>42</v>
       </c>
     </row>
     <row r="18" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A18" t="s">
-        <v>27</v>
+        <v>53</v>
       </c>
       <c r="B18" t="s">
         <v>8</v>
       </c>
-      <c r="C18" s="3" t="s">
-        <v>43</v>
+      <c r="C18" t="s">
+        <v>57</v>
       </c>
       <c r="D18" t="s">
         <v>9</v>
@@ -1073,20 +1076,17 @@
       </c>
       <c r="G18" t="s">
         <v>8</v>
-      </c>
-      <c r="H18" t="s">
-        <v>44</v>
       </c>
     </row>
     <row r="19" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A19" t="s">
-        <v>55</v>
+        <v>52</v>
       </c>
       <c r="B19" t="s">
         <v>8</v>
       </c>
       <c r="C19" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="D19" t="s">
         <v>9</v>
@@ -1103,13 +1103,13 @@
     </row>
     <row r="20" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A20" t="s">
-        <v>54</v>
+        <v>51</v>
       </c>
       <c r="B20" t="s">
         <v>8</v>
       </c>
       <c r="C20" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="D20" t="s">
         <v>9</v>
@@ -1126,13 +1126,13 @@
     </row>
     <row r="21" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A21" t="s">
-        <v>53</v>
+        <v>50</v>
       </c>
       <c r="B21" t="s">
         <v>8</v>
       </c>
       <c r="C21" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="D21" t="s">
         <v>9</v>
@@ -1145,17 +1145,20 @@
       </c>
       <c r="G21" t="s">
         <v>8</v>
+      </c>
+      <c r="H21" t="s">
+        <v>55</v>
       </c>
     </row>
     <row r="22" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A22" t="s">
-        <v>52</v>
+        <v>54</v>
       </c>
       <c r="B22" t="s">
         <v>8</v>
       </c>
       <c r="C22" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="D22" t="s">
         <v>9</v>
@@ -1170,18 +1173,18 @@
         <v>8</v>
       </c>
       <c r="H22" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
     </row>
     <row r="23" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A23" t="s">
-        <v>56</v>
+        <v>65</v>
       </c>
       <c r="B23" t="s">
         <v>8</v>
       </c>
       <c r="C23" t="s">
-        <v>63</v>
+        <v>49</v>
       </c>
       <c r="D23" t="s">
         <v>9</v>
@@ -1196,18 +1199,18 @@
         <v>8</v>
       </c>
       <c r="H23" t="s">
-        <v>58</v>
+        <v>64</v>
       </c>
     </row>
     <row r="24" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A24" t="s">
-        <v>67</v>
+        <v>63</v>
       </c>
       <c r="B24" t="s">
         <v>8</v>
       </c>
       <c r="C24" t="s">
-        <v>51</v>
+        <v>62</v>
       </c>
       <c r="D24" t="s">
         <v>9</v>
@@ -1216,24 +1219,21 @@
         <v>7</v>
       </c>
       <c r="F24" t="s">
-        <v>10</v>
+        <v>69</v>
       </c>
       <c r="G24" t="s">
         <v>8</v>
-      </c>
-      <c r="H24" t="s">
-        <v>66</v>
       </c>
     </row>
     <row r="25" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A25" t="s">
-        <v>65</v>
+        <v>67</v>
       </c>
       <c r="B25" t="s">
         <v>8</v>
       </c>
       <c r="C25" t="s">
-        <v>64</v>
+        <v>66</v>
       </c>
       <c r="D25" t="s">
         <v>9</v>
@@ -1242,21 +1242,24 @@
         <v>7</v>
       </c>
       <c r="F25" t="s">
-        <v>71</v>
+        <v>10</v>
       </c>
       <c r="G25" t="s">
         <v>8</v>
+      </c>
+      <c r="H25" t="s">
+        <v>68</v>
       </c>
     </row>
     <row r="26" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A26" t="s">
-        <v>69</v>
+        <v>70</v>
       </c>
       <c r="B26" t="s">
         <v>8</v>
       </c>
       <c r="C26" t="s">
-        <v>68</v>
+        <v>71</v>
       </c>
       <c r="D26" t="s">
         <v>9</v>
@@ -1269,32 +1272,32 @@
       </c>
       <c r="G26" t="s">
         <v>8</v>
-      </c>
-      <c r="H26" t="s">
-        <v>70</v>
       </c>
     </row>
     <row r="27" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A27" t="s">
+        <v>74</v>
+      </c>
+      <c r="B27" t="s">
+        <v>8</v>
+      </c>
+      <c r="C27" t="s">
         <v>72</v>
       </c>
-      <c r="B27" t="s">
-        <v>8</v>
-      </c>
-      <c r="C27" t="s">
+      <c r="D27" t="s">
+        <v>9</v>
+      </c>
+      <c r="E27" t="s">
+        <v>7</v>
+      </c>
+      <c r="F27" t="s">
+        <v>10</v>
+      </c>
+      <c r="G27" t="s">
+        <v>8</v>
+      </c>
+      <c r="H27" t="s">
         <v>73</v>
-      </c>
-      <c r="D27" t="s">
-        <v>9</v>
-      </c>
-      <c r="E27" t="s">
-        <v>7</v>
-      </c>
-      <c r="F27" t="s">
-        <v>10</v>
-      </c>
-      <c r="G27" t="s">
-        <v>8</v>
       </c>
     </row>
     <row r="28" spans="1:8" x14ac:dyDescent="0.35">
@@ -1305,7 +1308,7 @@
         <v>8</v>
       </c>
       <c r="C28" t="s">
-        <v>74</v>
+        <v>75</v>
       </c>
       <c r="D28" t="s">
         <v>9</v>
@@ -1320,7 +1323,7 @@
         <v>8</v>
       </c>
       <c r="H28" t="s">
-        <v>75</v>
+        <v>77</v>
       </c>
     </row>
     <row r="29" spans="1:8" x14ac:dyDescent="0.35">
@@ -1331,7 +1334,7 @@
         <v>8</v>
       </c>
       <c r="C29" t="s">
-        <v>77</v>
+        <v>79</v>
       </c>
       <c r="D29" t="s">
         <v>9</v>
@@ -1344,21 +1347,18 @@
       </c>
       <c r="G29" t="s">
         <v>8</v>
-      </c>
-      <c r="H29" t="s">
-        <v>79</v>
       </c>
     </row>
     <row r="30" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A30" t="s">
+        <v>81</v>
+      </c>
+      <c r="B30" t="s">
+        <v>8</v>
+      </c>
+      <c r="C30" t="s">
         <v>80</v>
       </c>
-      <c r="B30" t="s">
-        <v>8</v>
-      </c>
-      <c r="C30" t="s">
-        <v>81</v>
-      </c>
       <c r="D30" t="s">
         <v>9</v>
       </c>
@@ -1371,31 +1371,8 @@
       <c r="G30" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="31" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A31" t="s">
-        <v>83</v>
-      </c>
-      <c r="B31" t="s">
-        <v>8</v>
-      </c>
-      <c r="C31" t="s">
+      <c r="H30" t="s">
         <v>82</v>
-      </c>
-      <c r="D31" t="s">
-        <v>9</v>
-      </c>
-      <c r="E31" t="s">
-        <v>7</v>
-      </c>
-      <c r="F31" t="s">
-        <v>10</v>
-      </c>
-      <c r="G31" t="s">
-        <v>8</v>
-      </c>
-      <c r="H31" t="s">
-        <v>84</v>
       </c>
     </row>
   </sheetData>
@@ -1409,7 +1386,7 @@
   <dimension ref="C1:H17"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:H28"/>
+      <selection activeCell="A12" sqref="A12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>

</xml_diff>

<commit_message>
Implemented without double quotes logic
</commit_message>
<xml_diff>
--- a/src/main/resources/ScanTestData.xlsx
+++ b/src/main/resources/ScanTestData.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Automation Setup\AST Automation\Automation\src\main\resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{05594433-9493-4CC9-AAE1-E140FDCE219A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A4CEC921-DF93-40CA-9D16-FAA9D9A5E4ED}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="238" uniqueCount="83">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="223" uniqueCount="83">
   <si>
     <t>ScenarioDescription</t>
   </si>
@@ -658,7 +658,7 @@
   <dimension ref="A1:H30"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C15" sqref="C15"/>
+      <selection activeCell="B13" sqref="B13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1385,8 +1385,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C5771A20-F90E-4137-B244-FA403CC5F2C0}">
   <dimension ref="A1:H17"/>
   <sheetViews>
-    <sheetView topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:H3"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A6" sqref="A6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1422,53 +1422,7 @@
       </c>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A2" t="s">
-        <v>33</v>
-      </c>
-      <c r="B2" t="s">
-        <v>8</v>
-      </c>
-      <c r="C2" t="s">
-        <v>81</v>
-      </c>
-      <c r="D2" t="s">
-        <v>9</v>
-      </c>
-      <c r="E2" t="s">
-        <v>7</v>
-      </c>
-      <c r="F2" t="s">
-        <v>10</v>
-      </c>
-      <c r="G2" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A3" t="s">
-        <v>43</v>
-      </c>
-      <c r="B3" t="s">
-        <v>8</v>
-      </c>
-      <c r="C3" t="s">
-        <v>80</v>
-      </c>
-      <c r="D3" t="s">
-        <v>9</v>
-      </c>
-      <c r="E3" t="s">
-        <v>7</v>
-      </c>
-      <c r="F3" t="s">
-        <v>10</v>
-      </c>
-      <c r="G3" t="s">
-        <v>8</v>
-      </c>
-      <c r="H3" t="s">
-        <v>82</v>
-      </c>
+      <c r="C2" s="3"/>
     </row>
     <row r="15" spans="1:8" x14ac:dyDescent="0.35">
       <c r="C15" s="3"/>

</xml_diff>

<commit_message>
Application mapping Test cases
</commit_message>
<xml_diff>
--- a/src/main/resources/ScanTestData.xlsx
+++ b/src/main/resources/ScanTestData.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="29426"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="29530"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Automation Setup\AST Automation\Automation\src\main\resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A4CEC921-DF93-40CA-9D16-FAA9D9A5E4ED}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8EF6D2CB-6CB7-43B6-887D-5F4BF21D1739}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="170" windowWidth="19200" windowHeight="11110" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="ScanSheet" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="223" uniqueCount="83">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="239" uniqueCount="86">
   <si>
     <t>ScenarioDescription</t>
   </si>
@@ -105,18 +105,9 @@
     <t>containers</t>
   </si>
   <si>
-    <t>SAST scan with empty application name</t>
-  </si>
-  <si>
     <t>SAST scan with valid application name</t>
   </si>
   <si>
-    <t>SAST scan with invalid application name</t>
-  </si>
-  <si>
-    <t>`--application-name "ShubhamApplicationForAutomation"</t>
-  </si>
-  <si>
     <t>`--application-name ""</t>
   </si>
   <si>
@@ -150,9 +141,6 @@
     <t>SAST scan with Invalid sast-fast-scan flag</t>
   </si>
   <si>
-    <t>`--application-name "ApplicationForAutomation"</t>
-  </si>
-  <si>
     <t>provided application does not exist or user has no permission to the application</t>
   </si>
   <si>
@@ -283,6 +271,27 @@
   </si>
   <si>
     <t>Failed updating a project: Failed finding groups: [QA_Team_Invalid]</t>
+  </si>
+  <si>
+    <t>`--application-name "QAApplicationForAutomation"</t>
+  </si>
+  <si>
+    <t>`--application-name "InvaidApplicationForAutomation"</t>
+  </si>
+  <si>
+    <t>SAST scan with Valid Application Name</t>
+  </si>
+  <si>
+    <t>SAST scan with Invalid Application Name</t>
+  </si>
+  <si>
+    <t>SAST scan with Empty Application Name</t>
+  </si>
+  <si>
+    <t>`--application-name "QAApplicationForAutomation, CliAutomationApplication"</t>
+  </si>
+  <si>
+    <t>SAST scan with multipe Application in single command</t>
   </si>
 </sst>
 </file>
@@ -655,10 +664,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:H30"/>
+  <dimension ref="A1:H31"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B13" sqref="B13"/>
+      <selection activeCell="C10" sqref="C10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -692,12 +701,12 @@
         <v>11</v>
       </c>
       <c r="H1" s="2" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
-        <v>45</v>
+        <v>41</v>
       </c>
       <c r="B2" t="s">
         <v>8</v>
@@ -718,13 +727,13 @@
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
-        <v>44</v>
+        <v>40</v>
       </c>
       <c r="B3" t="s">
         <v>8</v>
       </c>
       <c r="C3" t="s">
-        <v>30</v>
+        <v>27</v>
       </c>
       <c r="D3" t="s">
         <v>9</v>
@@ -741,13 +750,13 @@
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
-        <v>32</v>
+        <v>29</v>
       </c>
       <c r="B4" t="s">
         <v>8</v>
       </c>
       <c r="C4" t="s">
-        <v>31</v>
+        <v>28</v>
       </c>
       <c r="D4" t="s">
         <v>9</v>
@@ -864,10 +873,10 @@
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A10" t="s">
-        <v>40</v>
+        <v>36</v>
       </c>
       <c r="B10" t="s">
-        <v>41</v>
+        <v>37</v>
       </c>
       <c r="D10" t="s">
         <v>9</v>
@@ -882,18 +891,18 @@
         <v>8</v>
       </c>
       <c r="H10" t="s">
-        <v>42</v>
+        <v>38</v>
       </c>
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A11" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
       <c r="B11" t="s">
         <v>8</v>
       </c>
       <c r="C11" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
       <c r="D11" t="s">
         <v>9</v>
@@ -910,13 +919,13 @@
     </row>
     <row r="12" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A12" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="B12" t="s">
         <v>8</v>
       </c>
       <c r="C12" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
       <c r="D12" t="s">
         <v>9</v>
@@ -931,18 +940,18 @@
         <v>8</v>
       </c>
       <c r="H12" t="s">
-        <v>35</v>
+        <v>32</v>
       </c>
     </row>
     <row r="13" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A13" t="s">
-        <v>33</v>
+        <v>30</v>
       </c>
       <c r="B13" t="s">
         <v>8</v>
       </c>
       <c r="C13" t="s">
-        <v>81</v>
+        <v>77</v>
       </c>
       <c r="D13" t="s">
         <v>9</v>
@@ -959,13 +968,13 @@
     </row>
     <row r="14" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A14" t="s">
-        <v>43</v>
+        <v>39</v>
       </c>
       <c r="B14" t="s">
         <v>8</v>
       </c>
       <c r="C14" t="s">
-        <v>80</v>
+        <v>76</v>
       </c>
       <c r="D14" t="s">
         <v>9</v>
@@ -980,18 +989,18 @@
         <v>8</v>
       </c>
       <c r="H14" t="s">
-        <v>82</v>
+        <v>78</v>
       </c>
     </row>
     <row r="15" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A15" t="s">
-        <v>23</v>
+        <v>83</v>
       </c>
       <c r="B15" t="s">
         <v>8</v>
       </c>
       <c r="C15" s="3" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
       <c r="D15" t="s">
         <v>9</v>
@@ -1008,13 +1017,13 @@
     </row>
     <row r="16" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A16" t="s">
-        <v>24</v>
+        <v>81</v>
       </c>
       <c r="B16" t="s">
         <v>8</v>
       </c>
       <c r="C16" s="3" t="s">
-        <v>26</v>
+        <v>79</v>
       </c>
       <c r="D16" t="s">
         <v>9</v>
@@ -1031,13 +1040,13 @@
     </row>
     <row r="17" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A17" t="s">
-        <v>25</v>
+        <v>85</v>
       </c>
       <c r="B17" t="s">
         <v>8</v>
       </c>
       <c r="C17" s="3" t="s">
-        <v>38</v>
+        <v>84</v>
       </c>
       <c r="D17" t="s">
         <v>9</v>
@@ -1052,18 +1061,18 @@
         <v>8</v>
       </c>
       <c r="H17" t="s">
-        <v>39</v>
+        <v>35</v>
       </c>
     </row>
     <row r="18" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A18" t="s">
-        <v>50</v>
+        <v>82</v>
       </c>
       <c r="B18" t="s">
         <v>8</v>
       </c>
-      <c r="C18" t="s">
-        <v>54</v>
+      <c r="C18" s="3" t="s">
+        <v>80</v>
       </c>
       <c r="D18" t="s">
         <v>9</v>
@@ -1076,17 +1085,20 @@
       </c>
       <c r="G18" t="s">
         <v>8</v>
+      </c>
+      <c r="H18" t="s">
+        <v>35</v>
       </c>
     </row>
     <row r="19" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A19" t="s">
-        <v>49</v>
+        <v>46</v>
       </c>
       <c r="B19" t="s">
         <v>8</v>
       </c>
       <c r="C19" t="s">
-        <v>55</v>
+        <v>50</v>
       </c>
       <c r="D19" t="s">
         <v>9</v>
@@ -1103,13 +1115,13 @@
     </row>
     <row r="20" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A20" t="s">
-        <v>48</v>
+        <v>45</v>
       </c>
       <c r="B20" t="s">
         <v>8</v>
       </c>
       <c r="C20" t="s">
-        <v>56</v>
+        <v>51</v>
       </c>
       <c r="D20" t="s">
         <v>9</v>
@@ -1126,13 +1138,13 @@
     </row>
     <row r="21" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A21" t="s">
-        <v>47</v>
+        <v>44</v>
       </c>
       <c r="B21" t="s">
         <v>8</v>
       </c>
       <c r="C21" t="s">
-        <v>57</v>
+        <v>52</v>
       </c>
       <c r="D21" t="s">
         <v>9</v>
@@ -1145,20 +1157,17 @@
       </c>
       <c r="G21" t="s">
         <v>8</v>
-      </c>
-      <c r="H21" t="s">
-        <v>52</v>
       </c>
     </row>
     <row r="22" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A22" t="s">
-        <v>51</v>
+        <v>43</v>
       </c>
       <c r="B22" t="s">
         <v>8</v>
       </c>
       <c r="C22" t="s">
-        <v>58</v>
+        <v>53</v>
       </c>
       <c r="D22" t="s">
         <v>9</v>
@@ -1173,18 +1182,18 @@
         <v>8</v>
       </c>
       <c r="H22" t="s">
-        <v>53</v>
+        <v>48</v>
       </c>
     </row>
     <row r="23" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A23" t="s">
-        <v>62</v>
+        <v>47</v>
       </c>
       <c r="B23" t="s">
         <v>8</v>
       </c>
       <c r="C23" t="s">
-        <v>46</v>
+        <v>54</v>
       </c>
       <c r="D23" t="s">
         <v>9</v>
@@ -1199,18 +1208,18 @@
         <v>8</v>
       </c>
       <c r="H23" t="s">
-        <v>61</v>
+        <v>49</v>
       </c>
     </row>
     <row r="24" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A24" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="B24" t="s">
         <v>8</v>
       </c>
       <c r="C24" t="s">
-        <v>59</v>
+        <v>42</v>
       </c>
       <c r="D24" t="s">
         <v>9</v>
@@ -1219,21 +1228,24 @@
         <v>7</v>
       </c>
       <c r="F24" t="s">
-        <v>66</v>
+        <v>10</v>
       </c>
       <c r="G24" t="s">
         <v>8</v>
+      </c>
+      <c r="H24" t="s">
+        <v>57</v>
       </c>
     </row>
     <row r="25" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A25" t="s">
-        <v>64</v>
+        <v>56</v>
       </c>
       <c r="B25" t="s">
         <v>8</v>
       </c>
       <c r="C25" t="s">
-        <v>63</v>
+        <v>55</v>
       </c>
       <c r="D25" t="s">
         <v>9</v>
@@ -1242,24 +1254,21 @@
         <v>7</v>
       </c>
       <c r="F25" t="s">
-        <v>10</v>
+        <v>62</v>
       </c>
       <c r="G25" t="s">
         <v>8</v>
-      </c>
-      <c r="H25" t="s">
-        <v>65</v>
       </c>
     </row>
     <row r="26" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A26" t="s">
-        <v>67</v>
+        <v>60</v>
       </c>
       <c r="B26" t="s">
         <v>8</v>
       </c>
       <c r="C26" t="s">
-        <v>68</v>
+        <v>59</v>
       </c>
       <c r="D26" t="s">
         <v>9</v>
@@ -1272,17 +1281,20 @@
       </c>
       <c r="G26" t="s">
         <v>8</v>
+      </c>
+      <c r="H26" t="s">
+        <v>61</v>
       </c>
     </row>
     <row r="27" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A27" t="s">
-        <v>71</v>
+        <v>63</v>
       </c>
       <c r="B27" t="s">
         <v>8</v>
       </c>
       <c r="C27" t="s">
-        <v>69</v>
+        <v>64</v>
       </c>
       <c r="D27" t="s">
         <v>9</v>
@@ -1295,20 +1307,17 @@
       </c>
       <c r="G27" t="s">
         <v>8</v>
-      </c>
-      <c r="H27" t="s">
-        <v>70</v>
       </c>
     </row>
     <row r="28" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A28" t="s">
-        <v>73</v>
+        <v>67</v>
       </c>
       <c r="B28" t="s">
         <v>8</v>
       </c>
       <c r="C28" t="s">
-        <v>72</v>
+        <v>65</v>
       </c>
       <c r="D28" t="s">
         <v>9</v>
@@ -1323,18 +1332,18 @@
         <v>8</v>
       </c>
       <c r="H28" t="s">
-        <v>74</v>
+        <v>66</v>
       </c>
     </row>
     <row r="29" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A29" t="s">
-        <v>75</v>
+        <v>69</v>
       </c>
       <c r="B29" t="s">
         <v>8</v>
       </c>
       <c r="C29" t="s">
-        <v>76</v>
+        <v>68</v>
       </c>
       <c r="D29" t="s">
         <v>9</v>
@@ -1347,17 +1356,20 @@
       </c>
       <c r="G29" t="s">
         <v>8</v>
+      </c>
+      <c r="H29" t="s">
+        <v>70</v>
       </c>
     </row>
     <row r="30" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A30" t="s">
-        <v>78</v>
+        <v>71</v>
       </c>
       <c r="B30" t="s">
         <v>8</v>
       </c>
       <c r="C30" t="s">
-        <v>77</v>
+        <v>72</v>
       </c>
       <c r="D30" t="s">
         <v>9</v>
@@ -1371,8 +1383,31 @@
       <c r="G30" t="s">
         <v>8</v>
       </c>
-      <c r="H30" t="s">
-        <v>79</v>
+    </row>
+    <row r="31" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A31" t="s">
+        <v>74</v>
+      </c>
+      <c r="B31" t="s">
+        <v>8</v>
+      </c>
+      <c r="C31" t="s">
+        <v>73</v>
+      </c>
+      <c r="D31" t="s">
+        <v>9</v>
+      </c>
+      <c r="E31" t="s">
+        <v>7</v>
+      </c>
+      <c r="F31" t="s">
+        <v>10</v>
+      </c>
+      <c r="G31" t="s">
+        <v>8</v>
+      </c>
+      <c r="H31" t="s">
+        <v>75</v>
       </c>
     </row>
   </sheetData>
@@ -1386,7 +1421,7 @@
   <dimension ref="A1:H17"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A6" sqref="A6"/>
+      <selection activeCell="B2" sqref="B2:H2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1418,11 +1453,34 @@
         <v>11</v>
       </c>
       <c r="H1" s="2" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="C2" s="3"/>
+      <c r="A2" t="s">
+        <v>23</v>
+      </c>
+      <c r="B2" t="s">
+        <v>8</v>
+      </c>
+      <c r="C2" s="3" t="s">
+        <v>84</v>
+      </c>
+      <c r="D2" t="s">
+        <v>9</v>
+      </c>
+      <c r="E2" t="s">
+        <v>7</v>
+      </c>
+      <c r="F2" t="s">
+        <v>10</v>
+      </c>
+      <c r="G2" t="s">
+        <v>8</v>
+      </c>
+      <c r="H2" t="s">
+        <v>35</v>
+      </c>
     </row>
     <row r="15" spans="1:8" x14ac:dyDescent="0.35">
       <c r="C15" s="3"/>
@@ -1435,5 +1493,6 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>